<commit_message>
Updated with 1.7.0 release
</commit_message>
<xml_diff>
--- a/rest-db-kafka/src/test/resources/event-xls/CreateUser-Event.xlsx
+++ b/rest-db-kafka/src/test/resources/event-xls/CreateUser-Event.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\rest-db-kafka\src\test\resources\event-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1C14AE-5FDE-4891-A893-BF3A7B1F1EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4003D76-F2DC-4314-B196-8E1D7C1F7818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserCreated-Event" sheetId="1" r:id="rId1"/>
+    <sheet name="SendUserMessage-Event" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -129,17 +130,51 @@
   </si>
   <si>
     <t xml:space="preserve">Create User </t>
+  </si>
+  <si>
+    <t>SEND_USER</t>
+  </si>
+  <si>
+    <t>VERIFY_USER_CREATED_EVENT_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @simple-kafka-send</t>
+  </si>
+  <si>
+    <t>Rockey</t>
+  </si>
+  <si>
+    <t>name,age
+Rockey,i~44</t>
+  </si>
+  <si>
+    <t>{ "name" : "Rocky","age":
+44 }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -287,34 +322,38 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -538,8 +577,8 @@
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -701,4 +740,128 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70F523B-26AE-4C0D-BA11-180407544A39}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="45" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>